<commit_message>
Cambios realizados para exponer + archivo notas
</commit_message>
<xml_diff>
--- a/BackEnd/Prueba.xlsx
+++ b/BackEnd/Prueba.xlsx
@@ -2584,11 +2584,7 @@
       </c>
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr"/>
-      <c r="W47" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="W47" t="inlineStr"/>
       <c r="X47" t="inlineStr"/>
     </row>
     <row r="48">

</xml_diff>